<commit_message>
change half of inventory
</commit_message>
<xml_diff>
--- a/modules/warehouse/uploads/file_sample/Sample_import_commodity_file_en.xlsx
+++ b/modules/warehouse/uploads/file_sample/Sample_import_commodity_file_en.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24729"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\sofware\perfex_webapp\branches\perfex_development\perfex_webapp\modules\warehouse\uploads\file_sample\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\ewc-\modules\warehouse\uploads\file_sample\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F914C024-516E-431E-95B0-BDA81B26A118}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13725"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t>Sku Code</t>
   </si>
@@ -48,9 +47,6 @@
     <t>Commodity Barcode</t>
   </si>
   <si>
-    <t>Sub group</t>
-  </si>
-  <si>
     <t>Warranty ( month )</t>
   </si>
   <si>
@@ -58,9 +54,6 @@
   </si>
   <si>
     <t>Unit</t>
-  </si>
-  <si>
-    <t>(*)Commodity Group</t>
   </si>
   <si>
     <t>Profit rate(%)</t>
@@ -146,11 +139,38 @@
       <t>Commodity Name</t>
     </r>
   </si>
+  <si>
+    <t>(*)Commodity Category</t>
+  </si>
+  <si>
+    <t>Sub Category</t>
+  </si>
+  <si>
+    <t>Length</t>
+  </si>
+  <si>
+    <t>Width</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Initail Quantity </t>
+  </si>
+  <si>
+    <t>Feet</t>
+  </si>
+  <si>
+    <t>Meters</t>
+  </si>
+  <si>
+    <t>Measurement</t>
+  </si>
+  <si>
+    <t>As Of Date</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -241,7 +261,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -260,6 +280,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -541,11 +564,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:V1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AC1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
+      <selection activeCell="AC1" sqref="AC1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -553,15 +576,21 @@
     <col min="1" max="19" width="33.5703125" style="1" customWidth="1"/>
     <col min="20" max="20" width="14.42578125" style="3" customWidth="1"/>
     <col min="21" max="22" width="22" style="3" customWidth="1"/>
-    <col min="23" max="16384" width="9.140625" style="3"/>
+    <col min="23" max="24" width="9.140625" style="3"/>
+    <col min="25" max="25" width="14.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="9.140625" style="3"/>
+    <col min="27" max="27" width="13.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="14.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="10.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="30" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" s="2" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:29" s="2" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>6</v>
@@ -573,55 +602,76 @@
         <v>1</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H1" s="4" t="s">
         <v>2</v>
       </c>
       <c r="I1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="L1" s="4" t="s">
         <v>10</v>
-      </c>
-      <c r="J1" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="K1" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="L1" s="4" t="s">
-        <v>12</v>
       </c>
       <c r="M1" s="4" t="s">
         <v>5</v>
       </c>
       <c r="N1" s="6" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="O1" s="4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="P1" s="4" t="s">
         <v>3</v>
       </c>
       <c r="Q1" s="4" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="R1" s="4" t="s">
         <v>4</v>
       </c>
       <c r="S1" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="T1" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="U1" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="V1" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="T1" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="U1" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="V1" s="5" t="s">
-        <v>17</v>
+      <c r="W1" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="X1" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y1" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="Z1" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="AA1" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="AB1" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="AC1" s="8" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>